<commit_message>
March 3 1041 pm
Completely revamped for NIST WEBBOOK operation only
</commit_message>
<xml_diff>
--- a/BinaryDistillationSimulator.xlsx
+++ b/BinaryDistillationSimulator.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\My Drive\PyScripts\ViaPy\distillation\equilibrium_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB53AEF-27C0-4AC2-BFEA-5E80B7C2759F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="13329" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Antoine" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -37,20 +43,50 @@
     <t>delta_H_vap_Tc</t>
   </si>
   <si>
-    <t>n-Decane</t>
+    <t>BP (K)</t>
+  </si>
+  <si>
+    <t>CpL</t>
   </si>
   <si>
     <t>Decane</t>
   </si>
   <si>
     <t>n-Octadecane</t>
+  </si>
+  <si>
+    <t>Butane</t>
+  </si>
+  <si>
+    <t>Pentane</t>
+  </si>
+  <si>
+    <t>heptane</t>
+  </si>
+  <si>
+    <t>dodecane</t>
+  </si>
+  <si>
+    <t>Ethane</t>
+  </si>
+  <si>
+    <t>Propane</t>
+  </si>
+  <si>
+    <t>Styrene</t>
+  </si>
+  <si>
+    <t>Propene</t>
+  </si>
+  <si>
+    <t>acetic acid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,13 +149,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -157,7 +201,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -191,6 +235,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -225,9 +270,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,14 +446,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.8984375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,10 +481,16 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>4.07857</v>
@@ -444,59 +502,71 @@
         <v>-78.67</v>
       </c>
       <c r="E2">
-        <v>51.23424439257924</v>
+        <v>51.234244392579242</v>
       </c>
       <c r="F2">
         <v>74.38</v>
       </c>
       <c r="G2">
-        <v>0.3238</v>
+        <v>0.32379999999999998</v>
       </c>
       <c r="H2">
         <v>617.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <v>447.2</v>
+      </c>
+      <c r="J2">
+        <v>313.86392857142857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>4.07857</v>
+        <v>4.33209</v>
       </c>
       <c r="C3">
-        <v>1501.268</v>
+        <v>2068.9630000000002</v>
       </c>
       <c r="D3">
-        <v>-78.67</v>
+        <v>-111.92700000000001</v>
       </c>
       <c r="E3">
-        <v>51.23424439257924</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="F3">
-        <v>74.38</v>
+        <v>-1</v>
       </c>
       <c r="G3">
-        <v>0.3238</v>
+        <v>-1</v>
       </c>
       <c r="H3">
-        <v>617.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>-1</v>
+      </c>
+      <c r="I3">
+        <v>589.29999999999995</v>
+      </c>
+      <c r="J3">
+        <v>566.20000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>4.33209</v>
+        <v>3.8500200000000002</v>
       </c>
       <c r="C4">
-        <v>2068.963</v>
+        <v>909.65</v>
       </c>
       <c r="D4">
-        <v>-111.927</v>
+        <v>-36.146000000000001</v>
       </c>
       <c r="E4">
-        <v>74.40000000000001</v>
+        <v>22.388999999999999</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -506,6 +576,268 @@
       </c>
       <c r="H4">
         <v>-1</v>
+      </c>
+      <c r="I4">
+        <v>273</v>
+      </c>
+      <c r="J4">
+        <v>131.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>3.9891999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1070.617</v>
+      </c>
+      <c r="D5">
+        <v>-40.454000000000001</v>
+      </c>
+      <c r="E5">
+        <v>18.694381273590778</v>
+      </c>
+      <c r="F5">
+        <v>37.01</v>
+      </c>
+      <c r="G5">
+        <v>0.41210000000000002</v>
+      </c>
+      <c r="H5">
+        <v>469.6</v>
+      </c>
+      <c r="I5">
+        <v>309.2</v>
+      </c>
+      <c r="J5">
+        <v>166.745</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>4.0283199999999999</v>
+      </c>
+      <c r="C6">
+        <v>1268.636</v>
+      </c>
+      <c r="D6">
+        <v>-56.198999999999998</v>
+      </c>
+      <c r="E6">
+        <v>36.452313919425748</v>
+      </c>
+      <c r="F6">
+        <v>53.66</v>
+      </c>
+      <c r="G6">
+        <v>0.28310000000000002</v>
+      </c>
+      <c r="H6">
+        <v>540.20000000000005</v>
+      </c>
+      <c r="I6">
+        <v>371.5</v>
+      </c>
+      <c r="J6">
+        <v>227.10163043478261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>4.1054899999999996</v>
+      </c>
+      <c r="C7">
+        <v>1625.9280000000001</v>
+      </c>
+      <c r="D7">
+        <v>-92.838999999999999</v>
+      </c>
+      <c r="E7">
+        <v>61.4</v>
+      </c>
+      <c r="F7">
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>489</v>
+      </c>
+      <c r="J7">
+        <v>374.67277777777792</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>3.9383499999999998</v>
+      </c>
+      <c r="C8">
+        <v>659.73900000000003</v>
+      </c>
+      <c r="D8">
+        <v>-16.719000000000001</v>
+      </c>
+      <c r="E8">
+        <v>4.6067892813398759</v>
+      </c>
+      <c r="F8">
+        <v>29.43</v>
+      </c>
+      <c r="G8">
+        <v>0.36959999999999998</v>
+      </c>
+      <c r="H8">
+        <v>305.39999999999998</v>
+      </c>
+      <c r="I8">
+        <v>184.6</v>
+      </c>
+      <c r="J8">
+        <v>70.460000000000008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>4.0115800000000004</v>
+      </c>
+      <c r="C9">
+        <v>834.26</v>
+      </c>
+      <c r="D9">
+        <v>-22.763000000000002</v>
+      </c>
+      <c r="E9">
+        <v>10.970329959506611</v>
+      </c>
+      <c r="F9">
+        <v>27.9</v>
+      </c>
+      <c r="G9">
+        <v>0.37659999999999999</v>
+      </c>
+      <c r="H9">
+        <v>369.8</v>
+      </c>
+      <c r="I9">
+        <v>231.1</v>
+      </c>
+      <c r="J9">
+        <v>105.4133333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>4.2194799999999999</v>
+      </c>
+      <c r="C10">
+        <v>1525.059</v>
+      </c>
+      <c r="D10">
+        <v>-56.378999999999998</v>
+      </c>
+      <c r="E10">
+        <v>42.5</v>
+      </c>
+      <c r="F10">
+        <v>-1</v>
+      </c>
+      <c r="G10">
+        <v>-1</v>
+      </c>
+      <c r="H10">
+        <v>-1</v>
+      </c>
+      <c r="I10">
+        <v>419</v>
+      </c>
+      <c r="J10">
+        <v>192.828</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>3.9748800000000002</v>
+      </c>
+      <c r="C11">
+        <v>795.81899999999996</v>
+      </c>
+      <c r="D11">
+        <v>-24.884</v>
+      </c>
+      <c r="E11">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="F11">
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <v>-1</v>
+      </c>
+      <c r="H11">
+        <v>-1</v>
+      </c>
+      <c r="I11">
+        <v>225.6</v>
+      </c>
+      <c r="J11">
+        <v>95.747500000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>4.6820599999999999</v>
+      </c>
+      <c r="C12">
+        <v>1642.54</v>
+      </c>
+      <c r="D12">
+        <v>-39.764000000000003</v>
+      </c>
+      <c r="E12">
+        <v>24.1316557138394</v>
+      </c>
+      <c r="F12">
+        <v>22.84</v>
+      </c>
+      <c r="G12">
+        <v>-4.5400000000000003E-2</v>
+      </c>
+      <c r="H12">
+        <v>592.70000000000005</v>
+      </c>
+      <c r="I12">
+        <v>391.2</v>
+      </c>
+      <c r="J12">
+        <v>131.03749999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
March 21 -- Working with NIST
Fixed a problem with the convergence of T.  This is now matching the results from the "old" version for butane/pentane.
</commit_message>
<xml_diff>
--- a/BinaryDistillationSimulator.xlsx
+++ b/BinaryDistillationSimulator.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\My Drive\PyScripts\ViaPy\distillation\equilibrium_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB53AEF-27C0-4AC2-BFEA-5E80B7C2759F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="13329" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Antoine" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>A</t>
   </si>
@@ -80,13 +74,61 @@
   </si>
   <si>
     <t>acetic acid</t>
+  </si>
+  <si>
+    <t>hexane</t>
+  </si>
+  <si>
+    <t>Hexane</t>
+  </si>
+  <si>
+    <t>ethanol</t>
+  </si>
+  <si>
+    <t>butanol</t>
+  </si>
+  <si>
+    <t>decane</t>
+  </si>
+  <si>
+    <t>pentane</t>
+  </si>
+  <si>
+    <t>butane</t>
+  </si>
+  <si>
+    <t>n-Butane</t>
+  </si>
+  <si>
+    <t>n-PEntane</t>
+  </si>
+  <si>
+    <t>n-Pentane</t>
+  </si>
+  <si>
+    <t>octane</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
+  <si>
+    <t>2-propanol</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>acetone</t>
+  </si>
+  <si>
+    <t>propanol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,21 +191,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +235,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -235,7 +269,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -270,10 +303,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,20 +478,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.8984375" customWidth="1"/>
-    <col min="5" max="5" width="21.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -488,7 +514,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -502,13 +528,13 @@
         <v>-78.67</v>
       </c>
       <c r="E2">
-        <v>51.234244392579242</v>
+        <v>51.23424439257924</v>
       </c>
       <c r="F2">
         <v>74.38</v>
       </c>
       <c r="G2">
-        <v>0.32379999999999998</v>
+        <v>0.3238</v>
       </c>
       <c r="H2">
         <v>617.4</v>
@@ -517,10 +543,10 @@
         <v>447.2</v>
       </c>
       <c r="J2">
-        <v>313.86392857142857</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <v>313.8639285714286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -528,13 +554,13 @@
         <v>4.33209</v>
       </c>
       <c r="C3">
-        <v>2068.9630000000002</v>
+        <v>2068.963</v>
       </c>
       <c r="D3">
-        <v>-111.92700000000001</v>
+        <v>-111.927</v>
       </c>
       <c r="E3">
-        <v>74.400000000000006</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -546,27 +572,27 @@
         <v>-1</v>
       </c>
       <c r="I3">
-        <v>589.29999999999995</v>
+        <v>589.3</v>
       </c>
       <c r="J3">
-        <v>566.20000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+        <v>566.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>3.8500200000000002</v>
+        <v>3.85002</v>
       </c>
       <c r="C4">
         <v>909.65</v>
       </c>
       <c r="D4">
-        <v>-36.146000000000001</v>
+        <v>-36.146</v>
       </c>
       <c r="E4">
-        <v>22.388999999999999</v>
+        <v>22.389</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -584,27 +610,27 @@
         <v>131.06</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5">
-        <v>3.9891999999999999</v>
+        <v>3.9892</v>
       </c>
       <c r="C5">
         <v>1070.617</v>
       </c>
       <c r="D5">
-        <v>-40.454000000000001</v>
+        <v>-40.454</v>
       </c>
       <c r="E5">
-        <v>18.694381273590778</v>
+        <v>18.69438127359078</v>
       </c>
       <c r="F5">
         <v>37.01</v>
       </c>
       <c r="G5">
-        <v>0.41210000000000002</v>
+        <v>0.4121</v>
       </c>
       <c r="H5">
         <v>469.6</v>
@@ -616,50 +642,50 @@
         <v>166.745</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6">
-        <v>4.0283199999999999</v>
+        <v>4.02832</v>
       </c>
       <c r="C6">
         <v>1268.636</v>
       </c>
       <c r="D6">
-        <v>-56.198999999999998</v>
+        <v>-56.199</v>
       </c>
       <c r="E6">
-        <v>36.452313919425748</v>
+        <v>36.45231391942575</v>
       </c>
       <c r="F6">
         <v>53.66</v>
       </c>
       <c r="G6">
-        <v>0.28310000000000002</v>
+        <v>0.2831</v>
       </c>
       <c r="H6">
-        <v>540.20000000000005</v>
+        <v>540.2</v>
       </c>
       <c r="I6">
         <v>371.5</v>
       </c>
       <c r="J6">
-        <v>227.10163043478261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>227.1016304347826</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B7">
-        <v>4.1054899999999996</v>
+        <v>4.10549</v>
       </c>
       <c r="C7">
-        <v>1625.9280000000001</v>
+        <v>1625.928</v>
       </c>
       <c r="D7">
-        <v>-92.838999999999999</v>
+        <v>-92.839</v>
       </c>
       <c r="E7">
         <v>61.4</v>
@@ -677,62 +703,62 @@
         <v>489</v>
       </c>
       <c r="J7">
-        <v>374.67277777777792</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>374.6727777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B8">
-        <v>3.9383499999999998</v>
+        <v>3.93835</v>
       </c>
       <c r="C8">
-        <v>659.73900000000003</v>
+        <v>659.739</v>
       </c>
       <c r="D8">
-        <v>-16.719000000000001</v>
+        <v>-16.719</v>
       </c>
       <c r="E8">
-        <v>4.6067892813398759</v>
+        <v>4.606789281339876</v>
       </c>
       <c r="F8">
         <v>29.43</v>
       </c>
       <c r="G8">
-        <v>0.36959999999999998</v>
+        <v>0.3696</v>
       </c>
       <c r="H8">
-        <v>305.39999999999998</v>
+        <v>305.4</v>
       </c>
       <c r="I8">
         <v>184.6</v>
       </c>
       <c r="J8">
-        <v>70.460000000000008</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>70.46000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9">
-        <v>4.0115800000000004</v>
+        <v>4.01158</v>
       </c>
       <c r="C9">
         <v>834.26</v>
       </c>
       <c r="D9">
-        <v>-22.763000000000002</v>
+        <v>-22.763</v>
       </c>
       <c r="E9">
-        <v>10.970329959506611</v>
+        <v>10.97032995950661</v>
       </c>
       <c r="F9">
         <v>27.9</v>
       </c>
       <c r="G9">
-        <v>0.37659999999999999</v>
+        <v>0.3766</v>
       </c>
       <c r="H9">
         <v>369.8</v>
@@ -744,18 +770,18 @@
         <v>105.4133333333333</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10">
-        <v>4.2194799999999999</v>
+        <v>4.21948</v>
       </c>
       <c r="C10">
         <v>1525.059</v>
       </c>
       <c r="D10">
-        <v>-56.378999999999998</v>
+        <v>-56.379</v>
       </c>
       <c r="E10">
         <v>42.5</v>
@@ -776,21 +802,21 @@
         <v>192.828</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11">
-        <v>3.9748800000000002</v>
+        <v>3.97488</v>
       </c>
       <c r="C11">
-        <v>795.81899999999996</v>
+        <v>795.819</v>
       </c>
       <c r="D11">
         <v>-24.884</v>
       </c>
       <c r="E11">
-        <v>18.420000000000002</v>
+        <v>18.42</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -805,21 +831,21 @@
         <v>225.6</v>
       </c>
       <c r="J11">
-        <v>95.747500000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>95.7475</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B12">
-        <v>4.6820599999999999</v>
+        <v>4.68206</v>
       </c>
       <c r="C12">
         <v>1642.54</v>
       </c>
       <c r="D12">
-        <v>-39.764000000000003</v>
+        <v>-39.764</v>
       </c>
       <c r="E12">
         <v>24.1316557138394</v>
@@ -828,16 +854,528 @@
         <v>22.84</v>
       </c>
       <c r="G12">
-        <v>-4.5400000000000003E-2</v>
+        <v>-0.0454</v>
       </c>
       <c r="H12">
-        <v>592.70000000000005</v>
+        <v>592.7</v>
       </c>
       <c r="I12">
         <v>391.2</v>
       </c>
       <c r="J12">
-        <v>131.03749999999999</v>
+        <v>131.0375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>4.00266</v>
+      </c>
+      <c r="C13">
+        <v>1171.53</v>
+      </c>
+      <c r="D13">
+        <v>-48.784</v>
+      </c>
+      <c r="E13">
+        <v>24.30962773413068</v>
+      </c>
+      <c r="F13">
+        <v>43.85</v>
+      </c>
+      <c r="G13">
+        <v>0.397</v>
+      </c>
+      <c r="H13">
+        <v>507.4</v>
+      </c>
+      <c r="I13">
+        <v>341.9</v>
+      </c>
+      <c r="J13">
+        <v>197.4310714285714</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>4.00266</v>
+      </c>
+      <c r="C14">
+        <v>1171.53</v>
+      </c>
+      <c r="D14">
+        <v>-48.784</v>
+      </c>
+      <c r="E14">
+        <v>24.30962773413068</v>
+      </c>
+      <c r="F14">
+        <v>43.85</v>
+      </c>
+      <c r="G14">
+        <v>0.397</v>
+      </c>
+      <c r="H14">
+        <v>507.4</v>
+      </c>
+      <c r="I14">
+        <v>341.9</v>
+      </c>
+      <c r="J14">
+        <v>197.4310714285714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5.37229</v>
+      </c>
+      <c r="C15">
+        <v>1670.409</v>
+      </c>
+      <c r="D15">
+        <v>-40.191</v>
+      </c>
+      <c r="E15">
+        <v>24.33819523365713</v>
+      </c>
+      <c r="F15">
+        <v>50.43</v>
+      </c>
+      <c r="G15">
+        <v>0.4989</v>
+      </c>
+      <c r="H15">
+        <v>513.9</v>
+      </c>
+      <c r="I15">
+        <v>351.5</v>
+      </c>
+      <c r="J15">
+        <v>113.1712121212121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>4.50393</v>
+      </c>
+      <c r="C16">
+        <v>1313.878</v>
+      </c>
+      <c r="D16">
+        <v>-98.789</v>
+      </c>
+      <c r="E16">
+        <v>25.4019450782909</v>
+      </c>
+      <c r="F16">
+        <v>62.53</v>
+      </c>
+      <c r="G16">
+        <v>0.696</v>
+      </c>
+      <c r="H16">
+        <v>562.9</v>
+      </c>
+      <c r="I16">
+        <v>390.6</v>
+      </c>
+      <c r="J16">
+        <v>181.1544444444445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>4.07857</v>
+      </c>
+      <c r="C17">
+        <v>1501.268</v>
+      </c>
+      <c r="D17">
+        <v>-78.67</v>
+      </c>
+      <c r="E17">
+        <v>51.23424439257924</v>
+      </c>
+      <c r="F17">
+        <v>74.38</v>
+      </c>
+      <c r="G17">
+        <v>0.3238</v>
+      </c>
+      <c r="H17">
+        <v>617.4</v>
+      </c>
+      <c r="I17">
+        <v>447.2</v>
+      </c>
+      <c r="J17">
+        <v>313.8639285714286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>3.9892</v>
+      </c>
+      <c r="C18">
+        <v>1070.617</v>
+      </c>
+      <c r="D18">
+        <v>-40.454</v>
+      </c>
+      <c r="E18">
+        <v>18.69438127359078</v>
+      </c>
+      <c r="F18">
+        <v>37.01</v>
+      </c>
+      <c r="G18">
+        <v>0.4121</v>
+      </c>
+      <c r="H18">
+        <v>469.6</v>
+      </c>
+      <c r="I18">
+        <v>309.2</v>
+      </c>
+      <c r="J18">
+        <v>166.745</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>3.85002</v>
+      </c>
+      <c r="C19">
+        <v>909.65</v>
+      </c>
+      <c r="D19">
+        <v>-36.146</v>
+      </c>
+      <c r="E19">
+        <v>22.389</v>
+      </c>
+      <c r="F19">
+        <v>-1</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>-1</v>
+      </c>
+      <c r="I19">
+        <v>273</v>
+      </c>
+      <c r="J19">
+        <v>131.06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>3.85002</v>
+      </c>
+      <c r="C20">
+        <v>909.65</v>
+      </c>
+      <c r="D20">
+        <v>-36.146</v>
+      </c>
+      <c r="E20">
+        <v>22.389</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>-1</v>
+      </c>
+      <c r="H20">
+        <v>-1</v>
+      </c>
+      <c r="I20">
+        <v>273</v>
+      </c>
+      <c r="J20">
+        <v>131.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>3.9892</v>
+      </c>
+      <c r="C21">
+        <v>1070.617</v>
+      </c>
+      <c r="D21">
+        <v>-40.454</v>
+      </c>
+      <c r="E21">
+        <v>18.69438127359078</v>
+      </c>
+      <c r="F21">
+        <v>37.01</v>
+      </c>
+      <c r="G21">
+        <v>0.4121</v>
+      </c>
+      <c r="H21">
+        <v>469.6</v>
+      </c>
+      <c r="I21">
+        <v>309.2</v>
+      </c>
+      <c r="J21">
+        <v>166.745</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>3.9892</v>
+      </c>
+      <c r="C22">
+        <v>1070.617</v>
+      </c>
+      <c r="D22">
+        <v>-40.454</v>
+      </c>
+      <c r="E22">
+        <v>18.69438127359078</v>
+      </c>
+      <c r="F22">
+        <v>37.01</v>
+      </c>
+      <c r="G22">
+        <v>0.4121</v>
+      </c>
+      <c r="H22">
+        <v>469.6</v>
+      </c>
+      <c r="I22">
+        <v>309.2</v>
+      </c>
+      <c r="J22">
+        <v>166.745</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>4.04867</v>
+      </c>
+      <c r="C23">
+        <v>1355.126</v>
+      </c>
+      <c r="D23">
+        <v>-63.633</v>
+      </c>
+      <c r="E23">
+        <v>38.23961950276017</v>
+      </c>
+      <c r="F23">
+        <v>58.46</v>
+      </c>
+      <c r="G23">
+        <v>0.3324</v>
+      </c>
+      <c r="H23">
+        <v>568.8</v>
+      </c>
+      <c r="I23">
+        <v>398.7</v>
+      </c>
+      <c r="J23">
+        <v>254.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>5.31301</v>
+      </c>
+      <c r="C24">
+        <v>1676.569</v>
+      </c>
+      <c r="D24">
+        <v>-21.728</v>
+      </c>
+      <c r="E24">
+        <v>24.33360839558782</v>
+      </c>
+      <c r="F24">
+        <v>45.3</v>
+      </c>
+      <c r="G24">
+        <v>0.4241</v>
+      </c>
+      <c r="H24">
+        <v>512.6</v>
+      </c>
+      <c r="I24">
+        <v>337.8</v>
+      </c>
+      <c r="J24">
+        <v>81.51269230769232</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>4.861</v>
+      </c>
+      <c r="C25">
+        <v>1357.427</v>
+      </c>
+      <c r="D25">
+        <v>-75.81399999999999</v>
+      </c>
+      <c r="E25">
+        <v>20.25317556886319</v>
+      </c>
+      <c r="F25">
+        <v>53.38</v>
+      </c>
+      <c r="G25">
+        <v>0.6538</v>
+      </c>
+      <c r="H25">
+        <v>508.3</v>
+      </c>
+      <c r="I25">
+        <v>355.5</v>
+      </c>
+      <c r="J25">
+        <v>162.1546666666667</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>3.55959</v>
+      </c>
+      <c r="C26">
+        <v>643.748</v>
+      </c>
+      <c r="D26">
+        <v>-198.043</v>
+      </c>
+      <c r="E26">
+        <v>40.65</v>
+      </c>
+      <c r="F26">
+        <v>40.65</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>373.17</v>
+      </c>
+      <c r="J26">
+        <v>75.348</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>4.42448</v>
+      </c>
+      <c r="C27">
+        <v>1312.253</v>
+      </c>
+      <c r="D27">
+        <v>-32.445</v>
+      </c>
+      <c r="E27">
+        <v>30.8789180453946</v>
+      </c>
+      <c r="F27">
+        <v>46.95</v>
+      </c>
+      <c r="G27">
+        <v>0.2826</v>
+      </c>
+      <c r="H27">
+        <v>508.2</v>
+      </c>
+      <c r="I27">
+        <v>329.3</v>
+      </c>
+      <c r="J27">
+        <v>125.8157142857143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>4.59871</v>
+      </c>
+      <c r="C28">
+        <v>1300.491</v>
+      </c>
+      <c r="D28">
+        <v>-86.364</v>
+      </c>
+      <c r="E28">
+        <v>20.15584124035262</v>
+      </c>
+      <c r="F28">
+        <v>52.06</v>
+      </c>
+      <c r="G28">
+        <v>0.6888</v>
+      </c>
+      <c r="H28">
+        <v>536.7</v>
+      </c>
+      <c r="I28">
+        <v>370.3</v>
+      </c>
+      <c r="J28">
+        <v>146.3658461538462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>